<commit_message>
Checkpoint commit of today's changes.
</commit_message>
<xml_diff>
--- a/is-prefix-of-string-in-table/Benchmark-05-v1.xlsx
+++ b/is-prefix-of-string-in-table/Benchmark-05-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Source\website\is-prefix-of-string-in-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3004017-81EC-45E4-AFD8-B0025E98849B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322AF75D-DC54-451A-868A-BE129A454B32}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="28425" xr2:uid="{B9DFE30A-EE13-47CA-8475-6F95B93D2FEE}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="155" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{047A855C-01F6-4FE1-B466-057F928FF933}" keepAlive="1" name="Query - release" description="Connection to the 'release' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - release" description="Connection to the 'release' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=release;Extended Properties=&quot;&quot;" command="SELECT * FROM [release]"/>
   </connection>
 </connections>
@@ -405,45 +405,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -526,45 +488,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -662,45 +586,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -785,49 +671,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="60000"/>
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="60000"/>
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="60000"/>
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1033,49 +877,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="60000"/>
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="60000"/>
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="60000"/>
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2682,7 +2484,7 @@
           <c:x val="0.66714993100089304"/>
           <c:y val="0.11098068927194014"/>
           <c:w val="0.3159593968279738"/>
-          <c:h val="7.5540630615062207E-2"/>
+          <c:h val="0.10973859465096382"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -9350,7 +9152,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05E1D70-7454-4DAF-87B2-1FBB002B8D78}" name="PivotTable5" cacheId="155" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05E1D70-7454-4DAF-87B2-1FBB002B8D78}" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:G25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -9826,7 +9628,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{F8F02154-F885-4CA2-A97B-603AAD1CF503}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="6">
     <queryTableFields count="5">
       <queryTableField id="1" name="Name" tableColumnId="1"/>

</xml_diff>